<commit_message>
All three testcases added
</commit_message>
<xml_diff>
--- a/testData/TestDataLogin.xlsx
+++ b/testData/TestDataLogin.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\eclipse-workspace\SpriteCloudAssignment\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC446FFB-6298-4E27-BC53-C824C7D0734A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{226176C4-8C20-4397-87D3-644D133275AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3624" yWindow="3360" windowWidth="13992" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
   <si>
     <t>Type</t>
   </si>
@@ -75,28 +75,28 @@
     <t>BlankUsername</t>
   </si>
   <si>
+    <t>InvalidPassword</t>
+  </si>
+  <si>
+    <t>demopass</t>
+  </si>
+  <si>
+    <t>performance_glitch_user</t>
+  </si>
+  <si>
+    <t>error_user</t>
+  </si>
+  <si>
+    <t>visual_user</t>
+  </si>
+  <si>
+    <t>BlankPassword</t>
+  </si>
+  <si>
+    <t>Epic sadface: Password is required</t>
+  </si>
+  <si>
     <t>Epic sadface: Username is required</t>
-  </si>
-  <si>
-    <t>InvalidPassword</t>
-  </si>
-  <si>
-    <t>demopass</t>
-  </si>
-  <si>
-    <t>performance_glitch_user</t>
-  </si>
-  <si>
-    <t>error_user</t>
-  </si>
-  <si>
-    <t>visual_user</t>
-  </si>
-  <si>
-    <t>BlankPassword</t>
-  </si>
-  <si>
-    <t>Epic sadface: Password is required</t>
   </si>
 </sst>
 </file>
@@ -444,8 +444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -535,18 +535,18 @@
         <v>6</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>13</v>
@@ -557,7 +557,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>6</v>
@@ -568,16 +568,14 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>7</v>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -585,7 +583,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>6</v>
@@ -595,24 +593,17 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
       <c r="C11" s="2"/>
-      <c r="D11" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="D11" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{4503875E-BCDC-4E22-ACD0-0F9A441570E9}"/>
     <hyperlink ref="D5" r:id="rId2" xr:uid="{9E7F9611-EE18-4242-94AF-29412DC2297E}"/>
     <hyperlink ref="D8" r:id="rId3" xr:uid="{58659992-AFF4-4A18-998D-B557D86001A3}"/>
-    <hyperlink ref="D9" r:id="rId4" xr:uid="{30F502BC-9C98-4270-A4BC-D187A6D25428}"/>
-    <hyperlink ref="D10" r:id="rId5" xr:uid="{0B215A79-42EA-430B-AFE1-3DACCE4C168F}"/>
+    <hyperlink ref="D10" r:id="rId4" xr:uid="{30F502BC-9C98-4270-A4BC-D187A6D25428}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>